<commit_message>
descriptieve analyse en significanties
</commit_message>
<xml_diff>
--- a/Data/Bronze/cornerballen2.xlsx
+++ b/Data/Bronze/cornerballen2.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cosyn\Desktop\thesis\thesis_code\Data\Bronze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A9410D-F2C1-4969-9610-1057269A75EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995FECB1-3A04-4758-ACD9-84CB3A6D0FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$604</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -1309,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q604"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E152" workbookViewId="0">
-      <selection activeCell="B159" sqref="A159:XFD162"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31737,6 +31740,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q604" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>